<commit_message>
Add new classes from CMR-QA: medical_imaging_study, imaging_scan_visit (renaming ScanVisit)
</commit_message>
<xml_diff>
--- a/data/metric_data-compare.xlsx
+++ b/data/metric_data-compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06d335bcba30d7c9/MSc Individual Project - SWT KG/iteration5/git-repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06d335bcba30d7c9/MSc Individual Project - SWT KG/iteration 9/git-repo/City-MSc-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{554943D4-5481-4C40-A9D1-4286F48FC2C7}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D53EBAC0-003F-46AE-87B8-3A1875FC0190}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,12 @@
     <sheet name="metrics_data-compare" sheetId="1" r:id="rId1"/>
     <sheet name="readme" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -1086,7 +1084,7 @@
   <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:X2"/>
+      <selection activeCell="M3" sqref="M3:V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,40 +1142,40 @@
         <v>13</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" t="s">
         <v>57</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" t="s">
         <v>11</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" t="s">
         <v>17</v>
       </c>
       <c r="Y2" s="2"/>

</xml_diff>

<commit_message>
tidy code for pasting into project report
</commit_message>
<xml_diff>
--- a/data/metric_data-compare.xlsx
+++ b/data/metric_data-compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06d335bcba30d7c9/MSc Individual Project - SWT KG/iteration10/git-repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C031C2AB-CAFA-4E06-8E8D-9C752A58DFBF}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{64AC38A9-2F7C-48E1-9E63-848BF6AFEB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F214D199-A538-4EAA-84DC-9D21C6782128}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -730,13 +730,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
@@ -1122,24 +1121,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI16"/>
+  <dimension ref="A1:AK16"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="3.5703125" style="3" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="24" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="3.5703125" style="3" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,110 +1152,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:37" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="Y2" s="2"/>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AD2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AH2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AI2" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1326,7 +1328,7 @@
         <f>IF(A3=M3,"match","error")</f>
         <v>match</v>
       </c>
-      <c r="AA3" s="5" t="str">
+      <c r="AA3" t="str">
         <f t="shared" ref="AA3:AI9" si="0">IF(B3=N3,"match","error")</f>
         <v>error</v>
       </c>
@@ -1363,7 +1365,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1434,7 +1436,7 @@
         <f t="shared" ref="Z4:Z9" si="1">IF(A4=M4,"match","error")</f>
         <v>match</v>
       </c>
-      <c r="AA4" s="5" t="str">
+      <c r="AA4" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1542,7 +1544,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA5" s="5" t="str">
+      <c r="AA5" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -1579,7 +1581,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1650,7 +1652,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA6" s="5" t="str">
+      <c r="AA6" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -1687,7 +1689,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1758,7 +1760,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA7" s="5" t="str">
+      <c r="AA7" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -1795,7 +1797,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1866,7 +1868,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA8" s="5" t="str">
+      <c r="AA8" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -1903,7 +1905,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1974,7 +1976,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="AA9" s="5" t="str">
+      <c r="AA9" t="str">
         <f t="shared" si="0"/>
         <v>error</v>
       </c>
@@ -2011,7 +2013,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2082,7 +2084,7 @@
         <f t="shared" ref="Z10:Z15" si="2">IF(A10=M10,"match","error")</f>
         <v>match</v>
       </c>
-      <c r="AA10" s="5" t="str">
+      <c r="AA10" t="str">
         <f t="shared" ref="AA10:AA15" si="3">IF(B10=N10,"match","error")</f>
         <v>error</v>
       </c>
@@ -2119,7 +2121,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2190,7 +2192,7 @@
         <f t="shared" si="2"/>
         <v>match</v>
       </c>
-      <c r="AA11" s="5" t="str">
+      <c r="AA11" t="str">
         <f t="shared" si="3"/>
         <v>error</v>
       </c>
@@ -2227,7 +2229,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2298,7 +2300,7 @@
         <f t="shared" si="2"/>
         <v>match</v>
       </c>
-      <c r="AA12" s="5" t="str">
+      <c r="AA12" t="str">
         <f t="shared" si="3"/>
         <v>error</v>
       </c>
@@ -2335,7 +2337,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2406,7 +2408,7 @@
         <f t="shared" si="2"/>
         <v>match</v>
       </c>
-      <c r="AA13" s="5" t="str">
+      <c r="AA13" t="str">
         <f t="shared" si="3"/>
         <v>error</v>
       </c>
@@ -2443,7 +2445,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2514,7 +2516,7 @@
         <f t="shared" si="2"/>
         <v>match</v>
       </c>
-      <c r="AA14" s="5" t="str">
+      <c r="AA14" t="str">
         <f t="shared" si="3"/>
         <v>error</v>
       </c>
@@ -2551,7 +2553,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2622,7 +2624,7 @@
         <f t="shared" si="2"/>
         <v>match</v>
       </c>
-      <c r="AA15" s="5" t="str">
+      <c r="AA15" t="str">
         <f t="shared" si="3"/>
         <v>error</v>
       </c>
@@ -2659,7 +2661,7 @@
         <v>match</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="AA16" t="s">
         <v>52</v>
       </c>
@@ -2674,15 +2676,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFD43F0-ACA6-43EC-8DB8-BD315A175ECB}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2691,37 +2695,37 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2866,29 +2870,29 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2989,29 +2993,29 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
@@ -3127,10 +3131,15 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD14"/>
+      <selection sqref="A1:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3138,33 +3147,33 @@
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3207,37 +3216,37 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -3286,53 +3295,53 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>IF(A3=A8,"match","ERROR")</f>
-        <v>match</v>
-      </c>
-      <c r="B13" s="7" t="str">
-        <f>IF(B3=B8,"match","ERROR")</f>
+        <f t="shared" ref="A13:F13" si="0">IF(A3=A8,"match","ERROR")</f>
+        <v>match</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f t="shared" si="0"/>
         <v>ERROR</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(C3=C8,"match","ERROR")</f>
+        <f t="shared" si="0"/>
         <v>match</v>
       </c>
       <c r="D13" t="str">
-        <f>IF(D3=D8,"match","ERROR")</f>
+        <f t="shared" si="0"/>
         <v>match</v>
       </c>
       <c r="E13" t="str">
-        <f>IF(E3=E8,"match","ERROR")</f>
+        <f t="shared" si="0"/>
         <v>match</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(F3=F8,"match","ERROR")</f>
+        <f t="shared" si="0"/>
         <v>match</v>
       </c>
     </row>
@@ -3346,10 +3355,17 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection sqref="A1:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3357,23 +3373,23 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -3590,25 +3606,25 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3705,9 +3721,9 @@
       <c r="G16">
         <v>2.9</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -3731,7 +3747,7 @@
       <c r="G17">
         <v>4</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -3762,19 +3778,19 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="F21" t="s">
@@ -3789,7 +3805,7 @@
         <f>IF(A3=A13,"match","ERROR")</f>
         <v>match</v>
       </c>
-      <c r="B22" s="7" t="str">
+      <c r="B22" s="6" t="str">
         <f t="shared" ref="B22:G22" si="0">IF(B3=B13,"match","ERROR")</f>
         <v>ERROR</v>
       </c>
@@ -3819,7 +3835,7 @@
         <f t="shared" ref="A23:G27" si="1">IF(A4=A14,"match","ERROR")</f>
         <v>match</v>
       </c>
-      <c r="B23" s="7" t="str">
+      <c r="B23" s="6" t="str">
         <f t="shared" si="1"/>
         <v>ERROR</v>
       </c>
@@ -3849,7 +3865,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="B24" s="7" t="str">
+      <c r="B24" s="6" t="str">
         <f t="shared" si="1"/>
         <v>ERROR</v>
       </c>
@@ -3879,7 +3895,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="B25" s="7" t="str">
+      <c r="B25" s="6" t="str">
         <f t="shared" si="1"/>
         <v>ERROR</v>
       </c>
@@ -3909,7 +3925,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="B26" s="7" t="str">
+      <c r="B26" s="6" t="str">
         <f t="shared" si="1"/>
         <v>ERROR</v>
       </c>
@@ -3939,7 +3955,7 @@
         <f t="shared" si="1"/>
         <v>match</v>
       </c>
-      <c r="B27" s="7" t="str">
+      <c r="B27" s="6" t="str">
         <f t="shared" si="1"/>
         <v>ERROR</v>
       </c>

</xml_diff>